<commit_message>
Prem | add route data files
</commit_message>
<xml_diff>
--- a/routedata/Balasore_PIS.xlsx
+++ b/routedata/Balasore_PIS.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanwisha.Mahapatra\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB869953-C87E-4590-A9B7-42D66F30E198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lot-1_36 Buses" sheetId="1" state="hidden" r:id="rId1"/>
@@ -19,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Nuapada!$A$3:$R$49</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="421">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -1304,12 +1298,15 @@
   </si>
   <si>
     <t>046</t>
+  </si>
+  <si>
+    <t>ଭାୟା- ଈଶ୍ୱରପୁର - କଣ୍ଡାଗରାଡ଼ି - ଶ୍ୟାମସୁନ୍ଦରପୁର -ଡାଖିନାରସିଂହପୁର -</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
@@ -1820,34 +1817,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.453125" customWidth="1"/>
-    <col min="8" max="8" width="19.54296875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.90625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.649999999999999" customHeight="1">
+    <row r="1" spans="1:9" ht="18.600000000000001" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2943,39 +2940,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28:H49"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O3" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" style="11" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" style="11"/>
-    <col min="4" max="4" width="13.54296875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="11" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="12.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.90625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="11" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="11"/>
+    <col min="4" max="4" width="13.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="11" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.85546875" style="11" customWidth="1"/>
     <col min="13" max="13" width="34" style="11" customWidth="1"/>
     <col min="14" max="14" width="78" style="11" customWidth="1"/>
-    <col min="15" max="15" width="68.1796875" style="11" customWidth="1"/>
-    <col min="16" max="16" width="18.81640625" style="11" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="16.54296875" style="11" hidden="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="11"/>
+    <col min="15" max="15" width="68.140625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" style="11" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="11" hidden="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="23">
+    <row r="1" spans="1:17" ht="23.25">
       <c r="A1" s="22" t="s">
         <v>174</v>
       </c>
@@ -2994,7 +2991,7 @@
       <c r="N1" s="22"/>
       <c r="O1" s="22"/>
     </row>
-    <row r="2" spans="1:17" ht="23">
+    <row r="2" spans="1:17" ht="23.25">
       <c r="A2" s="22" t="s">
         <v>173</v>
       </c>
@@ -3013,7 +3010,7 @@
       <c r="N2" s="22"/>
       <c r="O2" s="22"/>
     </row>
-    <row r="3" spans="1:17" ht="31">
+    <row r="3" spans="1:17" ht="31.5">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3112,7 +3109,7 @@
       <c r="P4" s="16"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17" ht="14.5" customHeight="1">
+    <row r="5" spans="1:17" ht="14.45" customHeight="1">
       <c r="A5" s="10">
         <v>2</v>
       </c>
@@ -3160,7 +3157,7 @@
       </c>
       <c r="Q5" s="10"/>
     </row>
-    <row r="6" spans="1:17" ht="31">
+    <row r="6" spans="1:17" ht="30">
       <c r="A6" s="10">
         <v>3</v>
       </c>
@@ -3298,7 +3295,7 @@
       <c r="P8" s="16"/>
       <c r="Q8" s="10"/>
     </row>
-    <row r="9" spans="1:17" ht="31">
+    <row r="9" spans="1:17" ht="30">
       <c r="A9" s="10">
         <v>6</v>
       </c>
@@ -3344,7 +3341,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="31">
+    <row r="10" spans="1:17" ht="30">
       <c r="A10" s="10">
         <v>7</v>
       </c>
@@ -3390,7 +3387,7 @@
       <c r="P10" s="16"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:17" ht="46.5">
+    <row r="11" spans="1:17" ht="45">
       <c r="A11" s="10">
         <v>8</v>
       </c>
@@ -3436,7 +3433,7 @@
       <c r="P11" s="19"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="12" spans="1:17" ht="77.5">
+    <row r="12" spans="1:17" ht="75">
       <c r="A12" s="10">
         <v>9</v>
       </c>
@@ -3480,7 +3477,7 @@
       <c r="P12" s="19"/>
       <c r="Q12" s="10"/>
     </row>
-    <row r="13" spans="1:17" ht="31">
+    <row r="13" spans="1:17" ht="30">
       <c r="A13" s="10">
         <v>10</v>
       </c>
@@ -3524,7 +3521,7 @@
       <c r="P13" s="19"/>
       <c r="Q13" s="10"/>
     </row>
-    <row r="14" spans="1:17" ht="46.5">
+    <row r="14" spans="1:17" ht="45">
       <c r="A14" s="10">
         <v>11</v>
       </c>
@@ -3568,7 +3565,7 @@
       <c r="P14" s="19"/>
       <c r="Q14" s="10"/>
     </row>
-    <row r="15" spans="1:17" ht="62">
+    <row r="15" spans="1:17" ht="60">
       <c r="A15" s="10">
         <v>12</v>
       </c>
@@ -3612,7 +3609,7 @@
       <c r="P15" s="19"/>
       <c r="Q15" s="10"/>
     </row>
-    <row r="16" spans="1:17" ht="46.5">
+    <row r="16" spans="1:17" ht="45">
       <c r="A16" s="10">
         <v>13</v>
       </c>
@@ -3656,7 +3653,7 @@
       <c r="P16" s="19"/>
       <c r="Q16" s="10"/>
     </row>
-    <row r="17" spans="1:17" ht="46.5">
+    <row r="17" spans="1:17" ht="45">
       <c r="A17" s="10">
         <v>14</v>
       </c>
@@ -3700,7 +3697,7 @@
       <c r="P17" s="19"/>
       <c r="Q17" s="10"/>
     </row>
-    <row r="18" spans="1:17" ht="31">
+    <row r="18" spans="1:17" ht="30">
       <c r="A18" s="10">
         <v>15</v>
       </c>
@@ -3744,7 +3741,7 @@
       <c r="P18" s="19"/>
       <c r="Q18" s="10"/>
     </row>
-    <row r="19" spans="1:17" ht="31">
+    <row r="19" spans="1:17" ht="30">
       <c r="A19" s="10">
         <v>16</v>
       </c>
@@ -3920,7 +3917,7 @@
       <c r="P22" s="19"/>
       <c r="Q22" s="10"/>
     </row>
-    <row r="23" spans="1:17" ht="31">
+    <row r="23" spans="1:17" ht="30">
       <c r="A23" s="10">
         <v>20</v>
       </c>
@@ -3964,7 +3961,7 @@
       <c r="P23" s="19"/>
       <c r="Q23" s="10"/>
     </row>
-    <row r="24" spans="1:17" ht="31">
+    <row r="24" spans="1:17" ht="30">
       <c r="A24" s="10">
         <v>21</v>
       </c>
@@ -4052,7 +4049,7 @@
       <c r="P25" s="19"/>
       <c r="Q25" s="10"/>
     </row>
-    <row r="26" spans="1:17" ht="31">
+    <row r="26" spans="1:17" ht="30">
       <c r="A26" s="10">
         <v>23</v>
       </c>
@@ -4096,7 +4093,7 @@
       <c r="P26" s="19"/>
       <c r="Q26" s="10"/>
     </row>
-    <row r="27" spans="1:17" ht="31">
+    <row r="27" spans="1:17" ht="45">
       <c r="A27" s="10">
         <v>24</v>
       </c>
@@ -4140,7 +4137,7 @@
       <c r="P27" s="19"/>
       <c r="Q27" s="10"/>
     </row>
-    <row r="28" spans="1:17" ht="62">
+    <row r="28" spans="1:17" ht="60">
       <c r="A28" s="10">
         <v>25</v>
       </c>
@@ -4184,7 +4181,7 @@
       <c r="P28" s="19"/>
       <c r="Q28" s="10"/>
     </row>
-    <row r="29" spans="1:17" ht="46.5">
+    <row r="29" spans="1:17" ht="45">
       <c r="A29" s="10">
         <v>26</v>
       </c>
@@ -4228,7 +4225,7 @@
       <c r="P29" s="19"/>
       <c r="Q29" s="10"/>
     </row>
-    <row r="30" spans="1:17" ht="31">
+    <row r="30" spans="1:17" ht="30">
       <c r="A30" s="10">
         <v>27</v>
       </c>
@@ -4272,7 +4269,7 @@
       <c r="P30" s="19"/>
       <c r="Q30" s="10"/>
     </row>
-    <row r="31" spans="1:17" ht="46.5">
+    <row r="31" spans="1:17" ht="45">
       <c r="A31" s="10">
         <v>28</v>
       </c>
@@ -4316,7 +4313,7 @@
       <c r="P31" s="19"/>
       <c r="Q31" s="10"/>
     </row>
-    <row r="32" spans="1:17" ht="62">
+    <row r="32" spans="1:17" ht="60">
       <c r="A32" s="10">
         <v>29</v>
       </c>
@@ -4360,7 +4357,7 @@
       <c r="P32" s="19"/>
       <c r="Q32" s="10"/>
     </row>
-    <row r="33" spans="1:17" ht="93">
+    <row r="33" spans="1:17" ht="105">
       <c r="A33" s="10">
         <v>30</v>
       </c>
@@ -4448,7 +4445,7 @@
       <c r="P34" s="19"/>
       <c r="Q34" s="10"/>
     </row>
-    <row r="35" spans="1:17" ht="31">
+    <row r="35" spans="1:17" ht="30">
       <c r="A35" s="10">
         <v>32</v>
       </c>
@@ -4536,7 +4533,7 @@
       <c r="P36" s="19"/>
       <c r="Q36" s="10"/>
     </row>
-    <row r="37" spans="1:17" ht="31">
+    <row r="37" spans="1:17" ht="30">
       <c r="A37" s="10">
         <v>34</v>
       </c>
@@ -4618,11 +4615,13 @@
       <c r="N38" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="O38" s="15"/>
+      <c r="O38" s="15" t="s">
+        <v>420</v>
+      </c>
       <c r="P38" s="19"/>
       <c r="Q38" s="10"/>
     </row>
-    <row r="39" spans="1:17" ht="46.5">
+    <row r="39" spans="1:17" ht="45">
       <c r="A39" s="10">
         <v>36</v>
       </c>
@@ -4666,7 +4665,7 @@
       <c r="P39" s="19"/>
       <c r="Q39" s="10"/>
     </row>
-    <row r="40" spans="1:17" ht="31">
+    <row r="40" spans="1:17" ht="30">
       <c r="A40" s="10">
         <v>37</v>
       </c>
@@ -4710,7 +4709,7 @@
       <c r="P40" s="19"/>
       <c r="Q40" s="10"/>
     </row>
-    <row r="41" spans="1:17" ht="46.5">
+    <row r="41" spans="1:17" ht="45">
       <c r="A41" s="10">
         <v>38</v>
       </c>
@@ -4754,7 +4753,7 @@
       <c r="P41" s="19"/>
       <c r="Q41" s="10"/>
     </row>
-    <row r="42" spans="1:17" ht="46.5">
+    <row r="42" spans="1:17" ht="45">
       <c r="A42" s="10">
         <v>39</v>
       </c>
@@ -4932,7 +4931,7 @@
       <c r="P45" s="19"/>
       <c r="Q45" s="10"/>
     </row>
-    <row r="46" spans="1:17" ht="31">
+    <row r="46" spans="1:17" ht="30">
       <c r="A46" s="10">
         <v>43</v>
       </c>
@@ -5064,7 +5063,7 @@
       <c r="P48" s="19"/>
       <c r="Q48" s="10"/>
     </row>
-    <row r="49" spans="1:17" ht="31">
+    <row r="49" spans="1:17" ht="30">
       <c r="A49" s="10">
         <v>46</v>
       </c>
@@ -5170,7 +5169,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="31">
+    <row r="52" spans="1:17" ht="30">
       <c r="A52" s="10">
         <v>48</v>
       </c>
@@ -5552,7 +5551,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:R49" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A3:R49"/>
   <mergeCells count="3">
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A1:O1"/>

</xml_diff>